<commit_message>
Topthread Percase Update w/ pid show up
</commit_message>
<xml_diff>
--- a/exitReview/Game_exitReview/Exit_Review_Top_Threads.xlsx
+++ b/exitReview/Game_exitReview/Exit_Review_Top_Threads.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="107">
   <si>
     <t>thread_1</t>
   </si>
@@ -47,7 +47,37 @@
     <t>value_5</t>
   </si>
   <si>
-    <t>Top5 Threads by total_insts_mill</t>
+    <t>thread_6</t>
+  </si>
+  <si>
+    <t>value_6</t>
+  </si>
+  <si>
+    <t>thread_7</t>
+  </si>
+  <si>
+    <t>value_7</t>
+  </si>
+  <si>
+    <t>thread_8</t>
+  </si>
+  <si>
+    <t>value_8</t>
+  </si>
+  <si>
+    <t>thread_9</t>
+  </si>
+  <si>
+    <t>value_9</t>
+  </si>
+  <si>
+    <t>thread_10</t>
+  </si>
+  <si>
+    <t>value_10</t>
+  </si>
+  <si>
+    <t>Top10 Threads by total_insts_mill</t>
   </si>
   <si>
     <t>GPHDR120</t>
@@ -65,40 +95,247 @@
     <t>ZZZVKLS01</t>
   </si>
   <si>
-    <t>Thread-</t>
-  </si>
-  <si>
-    <t>UnityMain</t>
-  </si>
-  <si>
-    <t>UnityGfxDeviceW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RenderThread </t>
-  </si>
-  <si>
-    <t>GameThread</t>
-  </si>
-  <si>
-    <t>RHIThread</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job.worker </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job.Worker </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TaskGraphNP </t>
-  </si>
-  <si>
-    <t>NativeThread</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TaskGraphHP </t>
-  </si>
-  <si>
-    <t>Background Job.</t>
+    <t>Thread-(sum_51)</t>
+  </si>
+  <si>
+    <t>UnityMain(sum_6)</t>
+  </si>
+  <si>
+    <t>UnityGfxDeviceW(32248)</t>
+  </si>
+  <si>
+    <t>RenderThread (10904)</t>
+  </si>
+  <si>
+    <t>UnityMain(sum_3)</t>
+  </si>
+  <si>
+    <t>Thread-(7418)</t>
+  </si>
+  <si>
+    <t>UnityMain(32522)</t>
+  </si>
+  <si>
+    <t>UnityMain(sum_4)</t>
+  </si>
+  <si>
+    <t>GameThread(sum_2)</t>
+  </si>
+  <si>
+    <t>UnityMain(26067)</t>
+  </si>
+  <si>
+    <t>RHIThread(7534)</t>
+  </si>
+  <si>
+    <t>Job.worker (sum_2)</t>
+  </si>
+  <si>
+    <t>UnityMain(32206)</t>
+  </si>
+  <si>
+    <t>GameThread(10684)</t>
+  </si>
+  <si>
+    <t>Job.Worker (sum_3)</t>
+  </si>
+  <si>
+    <t>RenderThread (7582)</t>
+  </si>
+  <si>
+    <t>UnityGfxDeviceW(400)</t>
+  </si>
+  <si>
+    <t>Job.Worker (sum_4)</t>
+  </si>
+  <si>
+    <t>RHIThread(10840)</t>
+  </si>
+  <si>
+    <t>UnityGfxDeviceW(26133)</t>
+  </si>
+  <si>
+    <t>TaskGraphNP (sum_5)</t>
+  </si>
+  <si>
+    <t>Job.worker (372)</t>
+  </si>
+  <si>
+    <t>NativeThread(sum_2)</t>
+  </si>
+  <si>
+    <t>TaskGraphHP (sum_3)</t>
+  </si>
+  <si>
+    <t>Background Job.(sum_15)</t>
+  </si>
+  <si>
+    <t>TaskGraphNP (7499)</t>
+  </si>
+  <si>
+    <t>Job.worker (371)</t>
+  </si>
+  <si>
+    <t>NativeThread(32254)</t>
+  </si>
+  <si>
+    <t>SRPSubmitThread(26130)</t>
+  </si>
+  <si>
+    <t>NativeThread(7529)</t>
+  </si>
+  <si>
+    <t>Thread-(sum_40)</t>
+  </si>
+  <si>
+    <t>Job.Worker (32238)</t>
+  </si>
+  <si>
+    <t>NativeThread(10883)</t>
+  </si>
+  <si>
+    <t>Job.Worker (26109)</t>
+  </si>
+  <si>
+    <t>TaskGraphNP (7500)</t>
+  </si>
+  <si>
+    <t>Job.Worker (32237)</t>
+  </si>
+  <si>
+    <t>TaskGraphHP (10785)</t>
+  </si>
+  <si>
+    <t>Job.Worker (26110)</t>
+  </si>
+  <si>
+    <t>surfaceflinger(sum_2)</t>
+  </si>
+  <si>
+    <t>NativeThread(3134)</t>
+  </si>
+  <si>
+    <t>Job.Worker (32235)</t>
+  </si>
+  <si>
+    <t>TaskGraphHP (10786)</t>
+  </si>
+  <si>
+    <t>Job.Worker (26111)</t>
+  </si>
+  <si>
+    <t>surfaceflinger(1867)</t>
+  </si>
+  <si>
+    <t>CoreThread(503)</t>
+  </si>
+  <si>
+    <t>Job.Worker (32236)</t>
+  </si>
+  <si>
+    <t>TaskGraphHP (10787)</t>
+  </si>
+  <si>
+    <t>Thread-(sum_45)</t>
+  </si>
+  <si>
+    <t>UnityGfxDeviceW(18349)</t>
+  </si>
+  <si>
+    <t>RenderThread (8177)</t>
+  </si>
+  <si>
+    <t>Thread-(6552)</t>
+  </si>
+  <si>
+    <t>UnityMain(29619)</t>
+  </si>
+  <si>
+    <t>UnityMain(13880)</t>
+  </si>
+  <si>
+    <t>RHIThread(6684)</t>
+  </si>
+  <si>
+    <t>UnityMain(18304)</t>
+  </si>
+  <si>
+    <t>GameThread(8028)</t>
+  </si>
+  <si>
+    <t>RenderThread (7135)</t>
+  </si>
+  <si>
+    <t>UnityGfxDeviceW(29677)</t>
+  </si>
+  <si>
+    <t>RHIThread(8146)</t>
+  </si>
+  <si>
+    <t>UnityGfxDeviceW(13927)</t>
+  </si>
+  <si>
+    <t>Job.worker (29669)</t>
+  </si>
+  <si>
+    <t>Job.Worker (13906)</t>
+  </si>
+  <si>
+    <t>TaskGraphNP (6632)</t>
+  </si>
+  <si>
+    <t>Job.worker (29668)</t>
+  </si>
+  <si>
+    <t>NativeThread(18354)</t>
+  </si>
+  <si>
+    <t>V DefaultWorke(sum_6)</t>
+  </si>
+  <si>
+    <t>Job.Worker (13905)</t>
+  </si>
+  <si>
+    <t>Job.Worker (18337)</t>
+  </si>
+  <si>
+    <t>TaskGraphHP (8120)</t>
+  </si>
+  <si>
+    <t>SRPSubmitThread(13925)</t>
+  </si>
+  <si>
+    <t>NativeThread(6676)</t>
+  </si>
+  <si>
+    <t>NativeThread(29861)</t>
+  </si>
+  <si>
+    <t>Job.Worker (18340)</t>
+  </si>
+  <si>
+    <t>TaskGraphNP (6633)</t>
+  </si>
+  <si>
+    <t>surfaceflinger(sum_3)</t>
+  </si>
+  <si>
+    <t>Job.Worker (18339)</t>
+  </si>
+  <si>
+    <t>NativeThread(8157)</t>
+  </si>
+  <si>
+    <t>Job.Worker (13904)</t>
+  </si>
+  <si>
+    <t>surfaceflinger(1864)</t>
+  </si>
+  <si>
+    <t>Job.Worker (18338)</t>
+  </si>
+  <si>
+    <t>V DefaultWorke(8164)</t>
   </si>
 </sst>
 </file>
@@ -456,15 +693,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -496,180 +733,360 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>35706.42</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <v>31526.34</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>28910.07</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="I2">
         <v>19899.96</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="K2">
         <v>13145.71</v>
       </c>
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2">
+        <v>7997.74</v>
+      </c>
+      <c r="N2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2">
+        <v>3725.49</v>
+      </c>
+      <c r="P2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2">
+        <v>2987.1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2">
+        <v>2647.34</v>
+      </c>
+      <c r="T2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2">
+        <v>2634.82</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>86978.95</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E3">
         <v>86855.44</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>50921.23</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="I3">
         <v>49384.45</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="K3">
         <v>28014.43</v>
       </c>
+      <c r="L3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3">
+        <v>22906.8</v>
+      </c>
+      <c r="N3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3">
+        <v>9477.370000000001</v>
+      </c>
+      <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3">
+        <v>9013.280000000001</v>
+      </c>
+      <c r="R3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3">
+        <v>9011.129999999999</v>
+      </c>
+      <c r="T3" t="s">
+        <v>70</v>
+      </c>
+      <c r="U3">
+        <v>4773.3</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>78431.14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>75421.03</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="G4">
         <v>75311.78</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I4">
         <v>69725.41</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="K4">
         <v>17860.58</v>
       </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4">
+        <v>17848.71</v>
+      </c>
+      <c r="N4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4">
+        <v>17631.81</v>
+      </c>
+      <c r="P4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4">
+        <v>17436.86</v>
+      </c>
+      <c r="R4" t="s">
+        <v>66</v>
+      </c>
+      <c r="S4">
+        <v>17427.12</v>
+      </c>
+      <c r="T4" t="s">
+        <v>71</v>
+      </c>
+      <c r="U4">
+        <v>17229.62</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>35489.66</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <v>35154.53</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G5">
         <v>35143.73</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="I5">
         <v>20485.51</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="K5">
         <v>17609.71</v>
       </c>
+      <c r="L5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5">
+        <v>8944.33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5">
+        <v>8941.559999999999</v>
+      </c>
+      <c r="P5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5">
+        <v>7074</v>
+      </c>
+      <c r="R5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5">
+        <v>5787.71</v>
+      </c>
+      <c r="T5" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5">
+        <v>4748</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:21">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>84302.49000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E6">
         <v>84281.91</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G6">
         <v>82461.77</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="I6">
         <v>50925.05</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="K6">
         <v>29577.06</v>
+      </c>
+      <c r="L6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M6">
+        <v>28050.94</v>
+      </c>
+      <c r="N6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6">
+        <v>27653.17</v>
+      </c>
+      <c r="P6" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q6">
+        <v>27444.93</v>
+      </c>
+      <c r="R6" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6">
+        <v>27363.68</v>
+      </c>
+      <c r="T6" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6">
+        <v>7362.36</v>
       </c>
     </row>
   </sheetData>
@@ -679,15 +1096,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -719,180 +1136,360 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="C2">
         <v>50702.9</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="E2">
         <v>44200.41</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="G2">
         <v>33860.34</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="I2">
         <v>26253.89</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="K2">
         <v>17888.6</v>
       </c>
+      <c r="L2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2">
+        <v>10638.48</v>
+      </c>
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2">
+        <v>6703.29</v>
+      </c>
+      <c r="P2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2">
+        <v>6702.57</v>
+      </c>
+      <c r="R2" t="s">
+        <v>99</v>
+      </c>
+      <c r="S2">
+        <v>4230.74</v>
+      </c>
+      <c r="T2" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2">
+        <v>2988.56</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>76825.89</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="E3">
         <v>76187</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>55476.23</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="I3">
         <v>52023.04</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="K3">
         <v>30412.99</v>
       </c>
+      <c r="L3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3">
+        <v>25063.25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3">
+        <v>8730.66</v>
+      </c>
+      <c r="P3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q3">
+        <v>8728.76</v>
+      </c>
+      <c r="R3" t="s">
+        <v>100</v>
+      </c>
+      <c r="S3">
+        <v>6779.07</v>
+      </c>
+      <c r="T3" t="s">
+        <v>104</v>
+      </c>
+      <c r="U3">
+        <v>6768.29</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>97334.72</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>83484.25999999999</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="G4">
         <v>83381.3</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I4">
         <v>70097.46000000001</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="K4">
         <v>18715.2</v>
       </c>
+      <c r="L4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4">
+        <v>18699</v>
+      </c>
+      <c r="N4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4">
+        <v>18316.91</v>
+      </c>
+      <c r="P4" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q4">
+        <v>17647.42</v>
+      </c>
+      <c r="R4" t="s">
+        <v>101</v>
+      </c>
+      <c r="S4">
+        <v>17121.94</v>
+      </c>
+      <c r="T4" t="s">
+        <v>105</v>
+      </c>
+      <c r="U4">
+        <v>17011.19</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C5">
         <v>37085.36</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <v>34712.85</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="G5">
         <v>34703.66</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="I5">
         <v>25661.25</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="K5">
         <v>17078.56</v>
       </c>
+      <c r="L5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5">
+        <v>13203.93</v>
+      </c>
+      <c r="N5" t="s">
+        <v>94</v>
+      </c>
+      <c r="O5">
+        <v>9439.26</v>
+      </c>
+      <c r="P5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5">
+        <v>8184.26</v>
+      </c>
+      <c r="R5" t="s">
+        <v>102</v>
+      </c>
+      <c r="S5">
+        <v>8182.71</v>
+      </c>
+      <c r="T5" t="s">
+        <v>106</v>
+      </c>
+      <c r="U5">
+        <v>5307.58</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:21">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>93585.06</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="E6">
         <v>93548.75999999999</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G6">
         <v>91964.71000000001</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="I6">
         <v>63936.12</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="K6">
         <v>30920.27</v>
+      </c>
+      <c r="L6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6">
+        <v>30812.51</v>
+      </c>
+      <c r="N6" t="s">
+        <v>95</v>
+      </c>
+      <c r="O6">
+        <v>30686.14</v>
+      </c>
+      <c r="P6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6">
+        <v>30351</v>
+      </c>
+      <c r="R6" t="s">
+        <v>103</v>
+      </c>
+      <c r="S6">
+        <v>30231.93</v>
+      </c>
+      <c r="T6" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6">
+        <v>8220.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>